<commit_message>
sincronizar database contratos com arquivo csv do comprasnetcontratos
</commit_message>
<xml_diff>
--- a/database/relatorio/PE 90041-2024/COMERCIAL_MINAS_BRASILIA_LTDA/relacao_itens.xlsx
+++ b/database/relatorio/PE 90041-2024/COMERCIAL_MINAS_BRASILIA_LTDA/relacao_itens.xlsx
@@ -439,14 +439,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 1 - CEMIPLIMABE (465440)</t>
+          <t>Grupo 1 - Item 1 - teste 1 (1)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>CEMIPLIMABE 350MG/7ML SOLUÇÃO PARA DILUIÇÃO PARA INFUSÃO</t>
+          <t>teste descricao detalhada 1</t>
         </is>
       </c>
     </row>
@@ -487,14 +487,14 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 2 - EVOLOCUMABE (439820)</t>
+          <t>Grupo 1 - Item 2 - teste 2 (2)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>EVOLOCUMABE 140 MG/ML SOLUÇÃO INJETÁVEL - SERINGA PREENCHIDA + CANETA APLICADORA</t>
+          <t>teste descricao detalhada 2</t>
         </is>
       </c>
     </row>
@@ -535,14 +535,14 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 3 - LENVATINIBE (448275)</t>
+          <t>Grupo 1 - Item 3 - teste 3 (3)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>LENVATINIBE 4MG CÁPSULA</t>
+          <t>teste descricao detalhada 3</t>
         </is>
       </c>
     </row>
@@ -583,14 +583,14 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 4 - LENVATINIBE (448276)</t>
+          <t>Grupo 1 - Item 4 - teste 4 (4)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>LENVATINIBE 10MG CÁPSULA</t>
+          <t>teste descricao detalhada 4</t>
         </is>
       </c>
     </row>
@@ -631,14 +631,14 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 5 - CLADRIBINA (483113)</t>
+          <t>Grupo 1 - Item 5 - teste 5 (5)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>CLADRIBINA 10MG COMPRIMIDO</t>
+          <t>teste descricao detalhada 5</t>
         </is>
       </c>
     </row>
@@ -679,14 +679,14 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 6 - LEVETIRACETAM (285965)</t>
+          <t>Grupo 1 - Item 6 - teste 6 (6)</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>LEVETIRACETAM 250MG COMPRIMIDO</t>
+          <t>teste descricao detalhada 6</t>
         </is>
       </c>
     </row>
@@ -727,14 +727,14 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 7 - SIROLIMO (285817)</t>
+          <t>Grupo 1 - Item 7 - teste 7 (7)</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>SIROLIMO 1MG COMPRIMIDO</t>
+          <t>teste descricao detalhada 7</t>
         </is>
       </c>
     </row>
@@ -775,14 +775,14 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 8 - RISDIPLAM (478939)</t>
+          <t>Grupo 1 - Item 8 - teste 8 (8)</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
-          <t>RISDIPLAM 0,75MG/ML X 80ML</t>
+          <t>teste descricao detalhada 8</t>
         </is>
       </c>
     </row>
@@ -823,14 +823,14 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 9 - SELEXIPAGUE (465388)</t>
+          <t>Grupo 1 - Item 9 - teste 9 (9)</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>SELEXIPAGUE 200MCG</t>
+          <t>teste descricao detalhada 9</t>
         </is>
       </c>
     </row>
@@ -871,14 +871,14 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 10 - SELEXIPAGUE (465385)</t>
+          <t>Grupo 1 - Item 10 - teste 10 (10)</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>SELEXIPAGUE 400MCG</t>
+          <t>teste descricao detalhada 10</t>
         </is>
       </c>
     </row>
@@ -919,14 +919,14 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 11 - POLATUZUMABE VEDOTINA (600809)</t>
+          <t>Grupo 1 - Item 11 - teste 11 (11)</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>POLATUZUMABE VEDOTINA 30MG PÓ LIOFILIZADO PARA SOLUÇÃO INJETÁVEL</t>
+          <t>teste descricao detalhada 11</t>
         </is>
       </c>
     </row>
@@ -967,14 +967,14 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 12 - POLATUZUMABE VEDOTINA (600810)</t>
+          <t>Grupo 1 - Item 12 - teste 12 (12)</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>POLATUZUMABE VEDOTINA 140MG PÓ LIOFILIZADO PARA SOLUÇÃO INJETÁVEL</t>
+          <t>teste descricao detalhada 12</t>
         </is>
       </c>
     </row>
@@ -1015,14 +1015,14 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 13 - CLORIDRATO DE BENDAMUSTINA (450760)</t>
+          <t>Grupo 1 - Item 13 - teste 13 (13)</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>CLORIDRATO DE BENDAMUSTINA 25MG FRASCO-AMPOLA</t>
+          <t>teste descricao detalhada 13</t>
         </is>
       </c>
     </row>
@@ -1063,14 +1063,14 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 14 - CLORIDRATO DE BENDAMUSTINA (428804)</t>
+          <t>Grupo 1 - Item 14 - teste 14 (14)</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>CLORIDRATO DE BENDAMUSTINA 100MG FRASCO-AMPOLA</t>
+          <t>teste descricao detalhada 14</t>
         </is>
       </c>
     </row>
@@ -1111,14 +1111,14 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 15 - IBRUTINIBE (430404)</t>
+          <t>Grupo 1 - Item 15 - teste 15 (15)</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>IBRUTINIBE 140MG COMPRIMIDO REVESTIDO</t>
+          <t>teste descricao detalhada 15</t>
         </is>
       </c>
     </row>
@@ -1159,14 +1159,14 @@
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 16 - CRIZOTINIBE (432637)</t>
+          <t>Grupo 1 - Item 16 - teste 16 (16)</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>CRIZOTINIBE 250MG CAPSULA</t>
+          <t>teste descricao detalhada 16</t>
         </is>
       </c>
     </row>
@@ -1207,14 +1207,14 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 17 - APIXABANA (429846)</t>
+          <t>Grupo 1 - Item 17 - teste 17 (17)</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>APIXABANA 5MG COMPRIMIDO</t>
+          <t>teste descricao detalhada 17</t>
         </is>
       </c>
     </row>
@@ -1255,14 +1255,14 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 18 - BECLOMETASONA (470130)</t>
+          <t>Grupo 1 - Item 18 - teste 18 (18)</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>BECLOMETASONA, DIPROPIONATO 100 MCG + FORMOTEROL DI-HIDRATADO, FUMARATO 6 MCG + GLICOPIRRÔNIO, BROMETO 12,5 MCG – SLUÇÃO AEROSSOL</t>
+          <t>teste descricao detalhada 18</t>
         </is>
       </c>
     </row>
@@ -1303,14 +1303,14 @@
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 19 - FOLINATO DE CÁLCIO (309041)</t>
+          <t>Grupo 1 - Item 19 - teste 19 (19)</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>FOLINATO DE CÁLCIO 300 MG (10MG/ML – 30ML)</t>
+          <t>teste descricao detalhada 19</t>
         </is>
       </c>
     </row>
@@ -1351,14 +1351,14 @@
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 20 - OLAPARIBE (458280)</t>
+          <t>Grupo 1 - Item 20 - teste 20 (20)</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>OLAPARIBE 150MG COMPRIMIDO</t>
+          <t>teste descricao detalhada 20</t>
         </is>
       </c>
     </row>
@@ -1399,14 +1399,14 @@
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 21 - PRAMIXEPOL (404612)</t>
+          <t>Grupo 1 - Item 21 - teste 21 (21)</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>PRAMIXEPOL 1,5MG LIBERAÇÃO PROLONGADA – COMPRIMIDO</t>
+          <t>teste descricao detalhada 21</t>
         </is>
       </c>
     </row>
@@ -1447,14 +1447,14 @@
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 22 - USTEQUINUMABE (400563)</t>
+          <t>Grupo 1 - Item 22 - teste 22 (22)</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>USTEQUINUMABE SOLUÇÃO INJETÁVEL 90MG/1,0ML SER (SC)</t>
+          <t>teste descricao detalhada 22</t>
         </is>
       </c>
     </row>
@@ -1495,14 +1495,14 @@
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 23 - USTEQUINUMABE (455395)</t>
+          <t>Grupo 1 - Item 23 - teste 23 (23)</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>USTEQUINUMABE SOLUÇÃO INJETÁVEL 130MG/26ML FRASCO-AMPOLA (IV)</t>
+          <t>teste descricao detalhada 23</t>
         </is>
       </c>
     </row>
@@ -1543,14 +1543,14 @@
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 24 - CLORETO DE RADIO (435439)</t>
+          <t>Grupo 1 - Item 24 - teste 24 (24)</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>CLORETO DE RADIO 223</t>
+          <t>teste descricao detalhada 24</t>
         </is>
       </c>
     </row>
@@ -1591,14 +1591,14 @@
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 25 - EXTRATO DE CÂNHAMO (468624)</t>
+          <t>Grupo 1 - Item 25 - teste 25 (25)</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>EXTRATO DE CÂNHAMO FULL SPRECTRUM – 50MG/ML DE CANABIDIOL – FR 100 ML (EQUIVALENTE A CHARLOTTE’S WEB)</t>
+          <t>teste descricao detalhada 25</t>
         </is>
       </c>
     </row>
@@ -1639,14 +1639,14 @@
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>Grupo 1 - Item 26 - ANIFROLUMABE (468624)</t>
+          <t>Grupo 1 - Item 26 - teste 26 (26)</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>ANIFROLUMABE 300 MG/2 ML – FRASCO-AMPOLA</t>
+          <t>teste descricao detalhada 26</t>
         </is>
       </c>
     </row>
@@ -1687,14 +1687,14 @@
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 27 - DASATINIBE (359135)</t>
+          <t>Grupo 2 - Item 27 - teste 27 (27)</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>DASATINIBE 20MG – COMPRIMIDO</t>
+          <t>teste descricao detalhada 27</t>
         </is>
       </c>
     </row>
@@ -1735,14 +1735,14 @@
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 28 - MAVACANTENO (359135)</t>
+          <t>Grupo 2 - Item 28 - teste 28 (28)</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>MAVACANTENO 5MG – CÁPSULA DURA</t>
+          <t>teste descricao detalhada 28</t>
         </is>
       </c>
     </row>
@@ -1783,14 +1783,14 @@
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 29 - LETERMOVIR (480035)</t>
+          <t>Grupo 2 - Item 29 - teste 29 (29)</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>LETERMOVIR 240MG – COMPRIMIDO REVESTIDO</t>
+          <t>teste descricao detalhada 29</t>
         </is>
       </c>
     </row>
@@ -1831,14 +1831,14 @@
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 30 - LETERMOVIR (480034)</t>
+          <t>Grupo 2 - Item 30 - teste 30 (30)</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="inlineStr">
         <is>
-          <t>LETERMOVIR 480MG - – COMPRIMIDO REVESTIDO</t>
+          <t>teste descricao detalhada 30</t>
         </is>
       </c>
     </row>
@@ -1879,14 +1879,14 @@
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 31 - POSACONAZOL (399995)</t>
+          <t>Grupo 2 - Item 31 - teste 31 (31)</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>POSACONAZOL 40MG/ML - FRASCO 105ML</t>
+          <t>teste descricao detalhada 31</t>
         </is>
       </c>
     </row>
@@ -1927,14 +1927,14 @@
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 32 - PEMETREXEDE (331938)</t>
+          <t>Grupo 2 - Item 32 - teste 32 (32)</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>PEMETREXEDE 500 mg</t>
+          <t>teste descricao detalhada 32</t>
         </is>
       </c>
     </row>
@@ -1975,14 +1975,14 @@
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 33 - BEVACIZUMABE (311390)</t>
+          <t>Grupo 2 - Item 33 - teste 33 (33)</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="2" t="inlineStr">
         <is>
-          <t>BEVACIZUMABE 400 MG SOLUÇÃO INJETÁVEL 25 MG/ML FRASCO-AMPOLA 16ML (IV)</t>
+          <t>teste descricao detalhada 33</t>
         </is>
       </c>
     </row>
@@ -2023,14 +2023,14 @@
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 34 - CICLOFOSFAMIDA (268427)</t>
+          <t>Grupo 2 - Item 34 - teste 34 (34)</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>CICLOFOSFAMIDA 50 MG</t>
+          <t>teste descricao detalhada 34</t>
         </is>
       </c>
     </row>
@@ -2071,14 +2071,14 @@
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 35 - DEFERASIROX (325837)</t>
+          <t>Grupo 2 - Item 35 - teste 35 (35)</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>DEFERASIROX 500 MG</t>
+          <t>teste descricao detalhada 35</t>
         </is>
       </c>
     </row>
@@ -2119,14 +2119,14 @@
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 36 - DEGARELIX (435231)</t>
+          <t>Grupo 2 - Item 36 - teste 36 (36)</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>DEGARELIX 80 MG</t>
+          <t>teste descricao detalhada 36</t>
         </is>
       </c>
     </row>
@@ -2167,14 +2167,14 @@
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 37 - DESMOPRESSINA (268074)</t>
+          <t>Grupo 2 - Item 37 - teste 37 (37)</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>DESMOPRESSINA ACETATO, DOSAGEM 0,1 MG/ML, SOLUÇÃO NASAL</t>
+          <t>teste descricao detalhada 37</t>
         </is>
       </c>
     </row>
@@ -2215,14 +2215,14 @@
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 38 - METOTREXATO (292249)</t>
+          <t>Grupo 2 - Item 38 - teste 38 (38)</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>METOTREXATO SOLUÇÃO INJETÁVEL 500MG (25MG/ML) FRASCO AMPOLA 20ML (IV)</t>
+          <t>teste descricao detalhada 38</t>
         </is>
       </c>
     </row>
@@ -2263,14 +2263,14 @@
     <row r="153">
       <c r="A153" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 39 - NUSINERSENA (439252)</t>
+          <t>Grupo 2 - Item 39 - teste 39 (39)</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>NUSINERSENA 2,4MG/ML SOL INJ 5ML</t>
+          <t>teste descricao detalhada 39</t>
         </is>
       </c>
     </row>
@@ -2311,14 +2311,14 @@
     <row r="157">
       <c r="A157" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 40 - PEGASPARGASE (443435)</t>
+          <t>Grupo 2 - Item 40 - teste 40 (40)</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="2" t="inlineStr">
         <is>
-          <t>PEGASPARGASE, CONCENTRAÇÃO 750 U/ML, FORMA FARMACÊUTICA SOLUÇÃO INJETÁVEL – 5ML</t>
+          <t>teste descricao detalhada 40</t>
         </is>
       </c>
     </row>
@@ -2359,14 +2359,14 @@
     <row r="161">
       <c r="A161" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 41 - PLERIXAFOR (413041)</t>
+          <t>Grupo 2 - Item 41 - teste 41 (41)</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="2" t="inlineStr">
         <is>
-          <t>PLERIXAFOR 20MG/ML, FRASCO-AMPOLA 1,2ML</t>
+          <t>teste descricao detalhada 41</t>
         </is>
       </c>
     </row>
@@ -2407,14 +2407,14 @@
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 42 - ROMOSOZUMABE (480015)</t>
+          <t>Grupo 2 - Item 42 - teste 42 (42)</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>ROMOSOZUMABE 90 MG/ML SOL INJ , SER 1,17 ML</t>
+          <t>teste descricao detalhada 42</t>
         </is>
       </c>
     </row>
@@ -2455,14 +2455,14 @@
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 43 - TERIPARATIDA (331223)</t>
+          <t>Grupo 2 - Item 43 - teste 43 (43)</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="2" t="inlineStr">
         <is>
-          <t>TERIPARATIDA SOLUÇÃO INJETÁVEL (250MCG/ML) CANETA 2,4ML (SC)</t>
+          <t>teste descricao detalhada 43</t>
         </is>
       </c>
     </row>
@@ -2503,14 +2503,14 @@
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 44 - TRETINOÍNA (278393)</t>
+          <t>Grupo 2 - Item 44 - teste 44 (44)</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>TRETINOÍNA 10MG CÁPSULA (VO)</t>
+          <t>teste descricao detalhada 44</t>
         </is>
       </c>
     </row>
@@ -2551,14 +2551,14 @@
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 45 - TRIÓXIDO (486455)</t>
+          <t>Grupo 2 - Item 45 - teste 45 (45)</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>TRIÓXIDO DE ARSÊNIO 2MG/ML, AMPOLA 6ML (IV)</t>
+          <t>teste descricao detalhada 45</t>
         </is>
       </c>
     </row>
@@ -2599,14 +2599,14 @@
     <row r="181">
       <c r="A181" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 46 - VENETOCLAX (450785)</t>
+          <t>Grupo 2 - Item 46 - teste 46 (46)</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>VENETOCLAX 100MG</t>
+          <t>teste descricao detalhada 46</t>
         </is>
       </c>
     </row>
@@ -2647,14 +2647,14 @@
     <row r="185">
       <c r="A185" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 47 - IMUNOGLOBULINA (343089)</t>
+          <t>Grupo 2 - Item 47 - teste 47 (47)</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>IMUNOGLOBULINA ANTITIMÓCITOS HUMANOS, TIPO DE COELHO, CONCENTRAÇÃO 25 MG, FORMA FARMACEUTICA PÓ LIÓFILO P/ INJETÁVEL</t>
+          <t>teste descricao detalhada 47</t>
         </is>
       </c>
     </row>
@@ -2695,14 +2695,14 @@
     <row r="189">
       <c r="A189" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 48 - CARBOPLATINA (270409)</t>
+          <t>Grupo 2 - Item 48 - teste 48 (48)</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="2" t="inlineStr">
         <is>
-          <t>CARBOPLATINA 450MG FRASCO-AMPOLA</t>
+          <t>teste descricao detalhada 48</t>
         </is>
       </c>
     </row>
@@ -2743,14 +2743,14 @@
     <row r="193">
       <c r="A193" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 49 - HIALURONATO DE SÓDIO (274467)</t>
+          <t>Grupo 2 - Item 49 - teste 49 (49)</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>HIALURONATO DE SÓDIO 1% (10MG/ML) – SER 2ML</t>
+          <t>teste descricao detalhada 49</t>
         </is>
       </c>
     </row>
@@ -2791,14 +2791,14 @@
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 50 - HIALURONATO DE SÓDIO (274467)</t>
+          <t>Grupo 2 - Item 50 - teste 50 (50)</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>HIALURONATO DE SÓDIO 1% (10MG/ML) – SER 2ML</t>
+          <t>teste descricao detalhada 50</t>
         </is>
       </c>
     </row>
@@ -2839,14 +2839,14 @@
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 51 - HIALURONATO DE SÓDIO (274467)</t>
+          <t>Grupo 2 - Item 51 - teste 51 (51)</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="2" t="inlineStr">
         <is>
-          <t>HIALURONATO DE SÓDIO 1% (10MG/ML) – SER 2ML</t>
+          <t>teste descricao detalhada 51</t>
         </is>
       </c>
     </row>
@@ -2887,14 +2887,14 @@
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>Grupo 2 - Item 52 - HIALURONATO DE SÓDIO (274467)</t>
+          <t>Grupo 2 - Item 52 - teste 52 (52)</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>HIALURONATO DE SÓDIO 1% (10MG/ML) – SER 2ML</t>
+          <t>teste descricao detalhada 52</t>
         </is>
       </c>
     </row>

</xml_diff>